<commit_message>
Add to Stock Done
</commit_message>
<xml_diff>
--- a/Database/Chick Fil A.xlsx
+++ b/Database/Chick Fil A.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Big StockRoom</t>
+          <t>Big Stockroom</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -458,11 +458,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>penunt oil</t>
+          <t>Penunt Oil</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>2021</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>1020</v>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
@@ -486,40 +486,6 @@
           <t>Y</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Rahul</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>13</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Rahul</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
All Done, Good Night
</commit_message>
<xml_diff>
--- a/Database/Chick Fil A.xlsx
+++ b/Database/Chick Fil A.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,39 +446,45 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Big Stockroom</t>
+          <t>Big StockRoom</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Small Stockroom</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Cooler</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Oil</t>
+          <t>Hashbrowns</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C2" t="inlineStr">
+        <v>50</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>M Box</t>
+          <t>Oil</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -486,15 +492,16 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>l box</t>
+          <t>Ketchup</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
@@ -502,54 +509,7 @@
           <t>Y</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ketchup</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>24</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Coater Spicy</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>coater</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>33</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>